<commit_message>
20190712-1958-lijw some support for images in settings.py and urls.py.
</commit_message>
<xml_diff>
--- a/数据库接口函数列表.xlsx
+++ b/数据库接口函数列表.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\WHU\curriculum\grade3-2\实训\python\TeamFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lijw\PycharmProjects\StudentAssosiationManagementPlatform\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17F86A51-AFC3-473A-96DD-B0FDA4807CD0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A0A6953-DDFA-4A45-8CDE-3F8BEBFDAB47}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="984" yWindow="-108" windowWidth="22164" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="50">
   <si>
     <t>输入</t>
   </si>
@@ -155,15 +155,6 @@
   </si>
   <si>
     <t>结果给出所有名称或ID包含搜索内容的社团的列表。若无则返回空列表，长度为零。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>字典result。
-字典result包括：
-    'success'-&gt;boolean，表示是否成功；//这个函数应该没有失败的情况吧
-    'notice'-&gt;String，表示提示信息，仅在result['success']为False时使用；
-    'number'-&gt;int，返回列表的长度，务必与实际列表长度一致；
-    'org_list'-&gt;List，列表中每项为一个(社团ID，社团名称，社团创建者)的tuple，tuple内为字符串类型</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -176,11 +167,71 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>若社团名org_name或社团ID被占用则失败。
+写入数据库时应同时写入成立时间、成立者、成员列表等。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串cookie_id，用于标识访问者；
+字符串org_id，表示社团ID，其中不含有非法字符；
+字符串org_name，表示社团名称；
+字符串org_description，表示社团描述信息；</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update_user_logo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update_org_logo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新个人头像</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新社团图标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串cookie_id；</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串cookie_id；
+文件imgfile = request.FILES['user_logo']。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get_user_logo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get_org_logo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>字符串cookie_id；
+文件imgfile （ = request.FILES['user_logo'] ）；
+字符串org_id，表示社团名称。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>读取个人头像</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>读取社团图标</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>字典result。
 字典result包括：
     'success'-&gt;boolean，是否成功；
     'notice'-&gt;String，提示信息，仅result['success']为False时使用。
     'info'-&gt;字典info，包括：
+        'user_name'-&gt;String；
         'gender'-&gt;String；
         'motto'-&gt;String；
         'birth_date'-&gt;datetime；
@@ -189,7 +240,52 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>字典result。
+    <t>字符串cookie_id；
+字符串org_id，表示社团名称。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">字典result。
+字典result包括：
+    'success'-&gt;boolean，是否成功；
+    'notice'-&gt;String，提示信息，仅在result['success']为False时使用；
+    'info'-&gt;字典info，包括：
+        'user_logo'-&gt;Image；
+        'user_name'-&gt;String，用户名。
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">字典result。
+字典result包括：
+    'success'-&gt;boolean，是否成功；
+    'notice'-&gt;String，提示信息，仅在result['success']为False时使用；
+    'info'-&gt;字典info，包括：
+        'org_logo'-&gt;Image；
+        'org_name'-&gt;String，社团名。
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">字典result。
+字典result包括：
+    'success'-&gt;boolean，是否成功；
+    'notice'-&gt;String，提示信息，仅在result['success']为False时使用；
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">字典result。
+字典result包括：
+    'success'-&gt;boolean，表示是否成功；//这个函数应该没有失败的情况吧
+    'notice'-&gt;String，表示提示信息，仅在result['success']为False时使用；
+    'number'-&gt;int，返回列表的长度，务必与实际列表长度一致；
+    'org_list'-&gt;List，列表中每项为一个(社团ID，社团名称，社团创建者)的tuple，tuple内为字符串类型
+</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">字典result。
 字典result包括：
     'success'-&gt;boolean，表示是否成功；
     'notice'-&gt;String，表示提示信息，仅在result['success']为False时使用；
@@ -199,19 +295,8 @@
         'create_date'-&gt;datetime，成立时间；
         'creator'-&gt;String，成立者用户名；
         'member_num'-&gt;int，成员人数。
-//后续可能添加社团管理者、社团审批等。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>若社团名org_name或社团ID被占用则失败。
-写入数据库时应同时写入成立时间、成立者、成员列表等。</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>字符串cookie_id，用于标识访问者；
-字符串org_id，表示社团ID，其中不含有非法字符；
-字符串org_name，表示社团名称；
-字符串org_description，表示社团描述信息；</t>
+//后续可能添加社团管理者、社团审批等。
+</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -219,7 +304,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -229,15 +314,6 @@
     </font>
     <font>
       <sz val="9"/>
-      <name val="等线"/>
-      <family val="3"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10.5"/>
-      <color theme="1"/>
       <name val="等线"/>
       <family val="3"/>
       <charset val="134"/>
@@ -288,19 +364,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -582,19 +652,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B2:F8"/>
+  <dimension ref="B2:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" thickBottom="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="18.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="11.6640625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="70.109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="69.21875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="32.5546875" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="2" width="18.33203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="70.109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="69.21875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="32.5546875" style="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6" thickBot="1" x14ac:dyDescent="0.3">
@@ -622,7 +692,7 @@
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>9</v>
@@ -631,7 +701,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="2:6" ht="152.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:6" ht="166.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
@@ -642,13 +712,13 @@
         <v>5</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>31</v>
+        <v>43</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:6" ht="97.2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:6" ht="132.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="1" t="s">
         <v>7</v>
       </c>
@@ -659,13 +729,13 @@
         <v>16</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="F5" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="2:6" ht="166.2" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:6" ht="180" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="1" t="s">
         <v>10</v>
       </c>
@@ -676,13 +746,13 @@
         <v>25</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="2:6" ht="83.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:6" ht="97.2" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="1" t="s">
         <v>17</v>
       </c>
@@ -690,30 +760,86 @@
         <v>18</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>19</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="2:6" ht="83.4" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="E8" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F8" s="4" t="s">
+      <c r="F8" s="1" t="s">
         <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" ht="69.599999999999994" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" ht="111" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B11" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" ht="111" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>